<commit_message>
Performance tests and results
</commit_message>
<xml_diff>
--- a/doc/CTC calculation v03.xlsx
+++ b/doc/CTC calculation v03.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haran\Documents\OpenSource\tfjsCtcLoss\tfjsctcloss\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFB19C7-F002-4DD5-870F-4A4DA3444956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141D8DC6-8128-4B7C-A4E9-B15B03F882E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="0" windowWidth="20895" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_C_A_" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -101,6 +102,21 @@
   <si>
     <t>TFJS gradient part
 (tensory method)</t>
+  </si>
+  <si>
+    <t>tensorflow</t>
+  </si>
+  <si>
+    <t>cpu</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>tf w. optimized JS impl.</t>
+  </si>
+  <si>
+    <t>cpu w. optimized JS impl.</t>
   </si>
 </sst>
 </file>
@@ -277,6 +293,1420 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU" b="1"/>
+              <a:t>Backend type and implementation impact on speed with different batch sizes</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="hu-HU" b="1" baseline="0"/>
+              <a:t> - CTC loss calculation</a:t>
+            </a:r>
+            <a:endParaRPr lang="hu-HU" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tensorflow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7990000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7510000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9440000000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7ED5-480D-BA3D-B53C750BCA18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cpu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0590000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2830000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7ED5-480D-BA3D-B53C750BCA18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tf w. optimized JS impl.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.651</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.411</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.641</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0379999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.827</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7ED5-480D-BA3D-B53C750BCA18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cpu w. optimized JS impl.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.76600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7120000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.383</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7ED5-480D-BA3D-B53C750BCA18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="455038472"/>
+        <c:axId val="455029616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="455038472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" b="1"/>
+                  <a:t>batch size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.92138656718006395"/>
+              <c:y val="0.92939027647347705"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455029616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="455029616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" b="1"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" b="1" baseline="0"/>
+                  <a:t> time (msec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455038472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1095374</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>42860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BEB026E-9474-4FA4-A681-05454A7AABCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -605,7 +2035,7 @@
   </sheetPr>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -1904,4 +3334,232 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D6D581-6F46-4CBA-A5AC-7A17B059B1D9}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>7.0990000000000002</v>
+      </c>
+      <c r="C2">
+        <v>1.663</v>
+      </c>
+      <c r="D2">
+        <v>1.651</v>
+      </c>
+      <c r="E2">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.7990000000000004</v>
+      </c>
+      <c r="C3">
+        <v>2.0590000000000002</v>
+      </c>
+      <c r="D3">
+        <v>1.536</v>
+      </c>
+      <c r="E3">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>6.7510000000000003</v>
+      </c>
+      <c r="C4">
+        <v>2.7189999999999999</v>
+      </c>
+      <c r="D4">
+        <v>1.411</v>
+      </c>
+      <c r="E4">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>6.9859999999999998</v>
+      </c>
+      <c r="C5">
+        <v>4.2830000000000004</v>
+      </c>
+      <c r="D5">
+        <v>1.641</v>
+      </c>
+      <c r="E5">
+        <v>1.5640000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>7.5229999999999997</v>
+      </c>
+      <c r="C6">
+        <v>7.3259999999999996</v>
+      </c>
+      <c r="D6">
+        <v>2.0379999999999998</v>
+      </c>
+      <c r="E6">
+        <v>2.7120000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>8.9440000000000008</v>
+      </c>
+      <c r="C7">
+        <v>13.693</v>
+      </c>
+      <c r="D7">
+        <v>2.827</v>
+      </c>
+      <c r="E7">
+        <v>5.383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>10.226000000000001</v>
+      </c>
+      <c r="C8">
+        <v>25.975999999999999</v>
+      </c>
+      <c r="D8">
+        <v>6.1719999999999997</v>
+      </c>
+      <c r="E8">
+        <v>9.9480000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>14.311</v>
+      </c>
+      <c r="C9">
+        <v>51.954000000000001</v>
+      </c>
+      <c r="D9">
+        <v>8.8640000000000008</v>
+      </c>
+      <c r="E9">
+        <v>20.994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="B10">
+        <v>22.77</v>
+      </c>
+      <c r="C10">
+        <v>103.94199999999999</v>
+      </c>
+      <c r="D10">
+        <v>16.138000000000002</v>
+      </c>
+      <c r="E10">
+        <v>44.863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>512</v>
+      </c>
+      <c r="B11">
+        <v>41.454999999999998</v>
+      </c>
+      <c r="C11">
+        <v>210.922</v>
+      </c>
+      <c r="D11">
+        <v>36.625999999999998</v>
+      </c>
+      <c r="E11">
+        <v>89.933000000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1024</v>
+      </c>
+      <c r="B12">
+        <v>90.382999999999996</v>
+      </c>
+      <c r="C12">
+        <v>433.42</v>
+      </c>
+      <c r="D12">
+        <v>85.509</v>
+      </c>
+      <c r="E12">
+        <v>197.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forward calculation cleanup, documentation update
</commit_message>
<xml_diff>
--- a/doc/CTC calculation v03.xlsx
+++ b/doc/CTC calculation v03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haran\Documents\OpenSource\tfjsCtcLoss\tfjsctcloss\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141D8DC6-8128-4B7C-A4E9-B15B03F882E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC913B10-86B2-457F-8E94-244A1CB8421D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -104,29 +104,30 @@
 (tensory method)</t>
   </si>
   <si>
-    <t>tensorflow</t>
-  </si>
-  <si>
-    <t>cpu</t>
-  </si>
-  <si>
     <t>Batch size</t>
   </si>
   <si>
-    <t>tf w. optimized JS impl.</t>
+    <t>tf-node w. TF impl.</t>
   </si>
   <si>
-    <t>cpu w. optimized JS impl.</t>
+    <t>JS w. TF impl.</t>
+  </si>
+  <si>
+    <t>tf-node w. Array impl.</t>
+  </si>
+  <si>
+    <t>JS w. Array impl.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -209,7 +210,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -234,6 +235,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -384,7 +386,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>tensorflow</c:v>
+                  <c:v>tf-node w. TF impl.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -415,10 +417,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:f>Performance!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -436,16 +438,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Performance!$B$2:$B$7</c:f>
+              <c:f>Performance!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>7.0990000000000002</c:v>
                 </c:pt>
@@ -463,6 +471,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.9440000000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.226000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.311</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,7 +497,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cpu</c:v>
+                  <c:v>JS w. TF impl.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -514,10 +528,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:f>Performance!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -535,16 +549,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Performance!$C$2:$C$7</c:f>
+              <c:f>Performance!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.663</c:v>
                 </c:pt>
@@ -562,6 +582,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>13.693</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.975999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51.954000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,7 +608,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>tf w. optimized JS impl.</c:v>
+                  <c:v>tf-node w. Array impl.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -613,10 +639,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:f>Performance!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -634,16 +660,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Performance!$D$2:$D$7</c:f>
+              <c:f>Performance!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.651</c:v>
                 </c:pt>
@@ -661,6 +693,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.827</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8640000000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -681,7 +719,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cpu w. optimized JS impl.</c:v>
+                  <c:v>JS w. Array impl.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -712,10 +750,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Performance!$A$2:$A$7</c:f>
+              <c:f>Performance!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -733,16 +771,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Performance!$E$2:$E$7</c:f>
+              <c:f>Performance!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.76600000000000001</c:v>
                 </c:pt>
@@ -760,6 +804,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9480000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,7 +1162,937 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU" sz="1400" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Backend type and implementation impact on batch item level speed with different batch sizes - CTC loss calculation</a:t>
+            </a:r>
+            <a:endParaRPr lang="hu-HU" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tf-node w. TF impl.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.0990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3995000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6877500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87324999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47018749999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15978125000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1118046875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8945312499999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ED24-4B56-A4C9-F1CDE7656925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JS w. TF impl.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0295000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67974999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53537500000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45787499999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42790624999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40587499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.405890625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40602343749999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ED24-4B56-A4C9-F1CDE7656925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tf-node w. Array impl.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.651</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35275000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.205125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12737499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8343749999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6437499999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.9250000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3039062500000007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ED24-4B56-A4C9-F1CDE7656925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JS w. Array impl.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.76600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23425000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16821875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15543750000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.164015625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17524609375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-ED24-4B56-A4C9-F1CDE7656925}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="619006440"/>
+        <c:axId val="619003488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="619006440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" b="1"/>
+                  <a:t>batch size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.9330942191220295"/>
+              <c:y val="0.93805795947570048"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619003488"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="619003488"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" b="1"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" b="1" baseline="0"/>
+                  <a:t> time (msec) per batch item</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619006440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1668,20 +2648,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1095374</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>42860</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>176210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1701,6 +3197,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B747A9D-05F3-4C34-A6D5-B8609DD9F189}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3338,30 +4870,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D6D581-6F46-4CBA-A5AC-7A17B059B1D9}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="Q53" sqref="Q53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>25</v>
@@ -3369,8 +4905,20 @@
       <c r="E1" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="F1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3386,8 +4934,24 @@
       <c r="E2">
         <v>0.76600000000000001</v>
       </c>
+      <c r="F2" s="14">
+        <f>B2/$A2</f>
+        <v>7.0990000000000002</v>
+      </c>
+      <c r="G2" s="14">
+        <f t="shared" ref="G2:I2" si="0">C2/$A2</f>
+        <v>1.663</v>
+      </c>
+      <c r="H2" s="14">
+        <f t="shared" si="0"/>
+        <v>1.651</v>
+      </c>
+      <c r="I2" s="14">
+        <f t="shared" si="0"/>
+        <v>0.76600000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3403,8 +4967,24 @@
       <c r="E3">
         <v>0.70799999999999996</v>
       </c>
+      <c r="F3" s="14">
+        <f t="shared" ref="F3:F12" si="1">B3/$A3</f>
+        <v>3.3995000000000002</v>
+      </c>
+      <c r="G3" s="14">
+        <f t="shared" ref="G3:G12" si="2">C3/$A3</f>
+        <v>1.0295000000000001</v>
+      </c>
+      <c r="H3" s="14">
+        <f t="shared" ref="H3:H12" si="3">D3/$A3</f>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I12" si="4">E3/$A3</f>
+        <v>0.35399999999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3420,8 +5000,24 @@
       <c r="E4">
         <v>0.93700000000000006</v>
       </c>
+      <c r="F4" s="14">
+        <f t="shared" si="1"/>
+        <v>1.6877500000000001</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" si="2"/>
+        <v>0.67974999999999997</v>
+      </c>
+      <c r="H4" s="14">
+        <f t="shared" si="3"/>
+        <v>0.35275000000000001</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="4"/>
+        <v>0.23425000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -3437,8 +5033,24 @@
       <c r="E5">
         <v>1.5640000000000001</v>
       </c>
+      <c r="F5" s="14">
+        <f t="shared" si="1"/>
+        <v>0.87324999999999997</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" si="2"/>
+        <v>0.53537500000000005</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" si="3"/>
+        <v>0.205125</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" si="4"/>
+        <v>0.19550000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
@@ -3454,8 +5066,24 @@
       <c r="E6">
         <v>2.7120000000000002</v>
       </c>
+      <c r="F6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.47018749999999998</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="2"/>
+        <v>0.45787499999999998</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="3"/>
+        <v>0.12737499999999999</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="4"/>
+        <v>0.16950000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>32</v>
       </c>
@@ -3471,8 +5099,24 @@
       <c r="E7">
         <v>5.383</v>
       </c>
+      <c r="F7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.27950000000000003</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="2"/>
+        <v>0.42790624999999999</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="3"/>
+        <v>8.8343749999999999E-2</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="4"/>
+        <v>0.16821875</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>64</v>
       </c>
@@ -3488,8 +5132,24 @@
       <c r="E8">
         <v>9.9480000000000004</v>
       </c>
+      <c r="F8" s="14">
+        <f t="shared" si="1"/>
+        <v>0.15978125000000001</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="2"/>
+        <v>0.40587499999999999</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="3"/>
+        <v>9.6437499999999995E-2</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="4"/>
+        <v>0.15543750000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>128</v>
       </c>
@@ -3505,8 +5165,24 @@
       <c r="E9">
         <v>20.994</v>
       </c>
+      <c r="F9" s="14">
+        <f t="shared" si="1"/>
+        <v>0.1118046875</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="2"/>
+        <v>0.405890625</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="3"/>
+        <v>6.9250000000000006E-2</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="4"/>
+        <v>0.164015625</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>256</v>
       </c>
@@ -3522,8 +5198,24 @@
       <c r="E10">
         <v>44.863</v>
       </c>
+      <c r="F10" s="14">
+        <f t="shared" si="1"/>
+        <v>8.8945312499999998E-2</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.40602343749999997</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="3"/>
+        <v>6.3039062500000007E-2</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="4"/>
+        <v>0.17524609375</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>512</v>
       </c>
@@ -3539,8 +5231,24 @@
       <c r="E11">
         <v>89.933000000000007</v>
       </c>
+      <c r="F11" s="14">
+        <f t="shared" si="1"/>
+        <v>8.0966796874999997E-2</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="2"/>
+        <v>0.41195703124999999</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="3"/>
+        <v>7.1535156249999995E-2</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="4"/>
+        <v>0.17565039062500001</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1024</v>
       </c>
@@ -3555,6 +5263,22 @@
       </c>
       <c r="E12">
         <v>197.19</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="1"/>
+        <v>8.8264648437499996E-2</v>
+      </c>
+      <c r="G12" s="14">
+        <f t="shared" si="2"/>
+        <v>0.42326171875000002</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="3"/>
+        <v>8.35048828125E-2</v>
+      </c>
+      <c r="I12" s="14">
+        <f t="shared" si="4"/>
+        <v>0.192568359375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>